<commit_message>
Criação do arquivo MonthReport.xlsx consolidando os arquivos de entrada Sales.xlsx e Acquisitions.xlsx Criação e calculo de duas colunas na planilha Sales de MonthReport: "Total Sales" e "Froft Per Sale" Formatação da planilha Sales como Tabela Criação de uma Planilha Dinãmica mostranto "Total Sales" e "Froft Per Sale" por "Agent Name"
</commit_message>
<xml_diff>
--- a/Data/Input/Acquisitions.xlsx
+++ b/Data/Input/Acquisitions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Adriano\Meus Arquivos\UiPath\Projetos\UipathAcademy\BasicProjects\ExcelDataConsolidation\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04EB61D-05B1-4856-BE75-9DAD536415F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CE50CD-2C9F-4E47-9CE9-7C9F39C73DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="23040" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="23040" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisitions" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Acrescenta um gráfico de barras para ilustrar as informações da Tabela Dinâmica
</commit_message>
<xml_diff>
--- a/Data/Input/Acquisitions.xlsx
+++ b/Data/Input/Acquisitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Adriano\Meus Arquivos\UiPath\Projetos\UipathAcademy\BasicProjects\ExcelDataConsolidation\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CE50CD-2C9F-4E47-9CE9-7C9F39C73DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E563E76B-A2CE-41CD-98CB-CC9492714E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="732" yWindow="732" windowWidth="23040" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1822,6 +1822,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="34d2ab49-b14c-40af-8c3f-b2a27eb69e13" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="328982d7-d2af-46e2-9ab4-9b069b3e82d0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B47328280439544AB5C41C56297158F8" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="50e5b6106be706602d4845c0a9b0c3da">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="825ee06b-ca9e-4fae-a309-081319cc5c11" xmlns:ns3="328982d7-d2af-46e2-9ab4-9b069b3e82d0" xmlns:ns4="34d2ab49-b14c-40af-8c3f-b2a27eb69e13" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f931b1fd44a63a33fbd98fb4653837c7" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="825ee06b-ca9e-4fae-a309-081319cc5c11"/>
@@ -2063,17 +2074,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="34d2ab49-b14c-40af-8c3f-b2a27eb69e13" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="328982d7-d2af-46e2-9ab4-9b069b3e82d0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2084,6 +2084,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB5C6EBF-4902-4536-B72A-0466FB8219D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="34d2ab49-b14c-40af-8c3f-b2a27eb69e13"/>
+    <ds:schemaRef ds:uri="328982d7-d2af-46e2-9ab4-9b069b3e82d0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFAAA239-A697-4242-BDF8-153903A180C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2103,17 +2114,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB5C6EBF-4902-4536-B72A-0466FB8219D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="34d2ab49-b14c-40af-8c3f-b2a27eb69e13"/>
-    <ds:schemaRef ds:uri="328982d7-d2af-46e2-9ab4-9b069b3e82d0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AB9A8E1-E04D-4628-9179-505861E9CEB4}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Acrescenta proteção com senha nas planilhas "Sales" e "Pivot Table"
</commit_message>
<xml_diff>
--- a/Data/Input/Acquisitions.xlsx
+++ b/Data/Input/Acquisitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Adriano\Meus Arquivos\UiPath\Projetos\UipathAcademy\BasicProjects\ExcelDataConsolidation\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E563E76B-A2CE-41CD-98CB-CC9492714E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2176FE2B-C108-41A6-A949-7B0BE3E5A5EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="732" yWindow="732" windowWidth="23040" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1822,17 +1822,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="34d2ab49-b14c-40af-8c3f-b2a27eb69e13" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="328982d7-d2af-46e2-9ab4-9b069b3e82d0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B47328280439544AB5C41C56297158F8" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="50e5b6106be706602d4845c0a9b0c3da">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="825ee06b-ca9e-4fae-a309-081319cc5c11" xmlns:ns3="328982d7-d2af-46e2-9ab4-9b069b3e82d0" xmlns:ns4="34d2ab49-b14c-40af-8c3f-b2a27eb69e13" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f931b1fd44a63a33fbd98fb4653837c7" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="825ee06b-ca9e-4fae-a309-081319cc5c11"/>
@@ -2074,6 +2063,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="34d2ab49-b14c-40af-8c3f-b2a27eb69e13" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="328982d7-d2af-46e2-9ab4-9b069b3e82d0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2084,17 +2084,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB5C6EBF-4902-4536-B72A-0466FB8219D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="34d2ab49-b14c-40af-8c3f-b2a27eb69e13"/>
-    <ds:schemaRef ds:uri="328982d7-d2af-46e2-9ab4-9b069b3e82d0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CFAAA239-A697-4242-BDF8-153903A180C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2114,6 +2103,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB5C6EBF-4902-4536-B72A-0466FB8219D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="34d2ab49-b14c-40af-8c3f-b2a27eb69e13"/>
+    <ds:schemaRef ds:uri="328982d7-d2af-46e2-9ab4-9b069b3e82d0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AB9A8E1-E04D-4628-9179-505861E9CEB4}">
   <ds:schemaRefs>

</xml_diff>